<commit_message>
WIP Demographics data and descriptives
</commit_message>
<xml_diff>
--- a/badbaby/static/badbaby_final_121818.xlsx
+++ b/badbaby/static/badbaby_final_121818.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="459">
   <si>
     <t xml:space="preserve">2 months-old</t>
   </si>
@@ -1279,9 +1279,6 @@
   </si>
   <si>
     <t xml:space="preserve">Epoching fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U</t>
   </si>
   <si>
     <t xml:space="preserve">8 lbs 2 ozs</t>
@@ -1417,14 +1414,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="169" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="170" formatCode="MMM\-YY"/>
+    <numFmt numFmtId="169" formatCode="MMM\-YY"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -2033,7 +2029,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2049,7 +2045,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2255,13 +2251,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="24.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="24.34"/>
   </cols>
   <sheetData>
@@ -3416,7 +3412,7 @@
     <row r="31" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="str">
         <f aca="false">" N = "&amp;COUNTA(A2:A30)</f>
-        <v> N = 29</v>
+        <v>N = 29</v>
       </c>
       <c r="B31" s="29" t="str">
         <f aca="false">COUNTIF(B2:B30,"M")&amp;" Males; "&amp;COUNTIF(B2:B30,"F")&amp;" Females"</f>
@@ -4617,7 +4613,7 @@
     <row r="63" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="str">
         <f aca="false">" N = "&amp;COUNTA(A32:A62)</f>
-        <v> N = 31</v>
+        <v>N = 31</v>
       </c>
       <c r="B63" s="29" t="str">
         <f aca="false">COUNTIF(B32:B62,"M")&amp;" Males; "&amp;COUNTIF(B32:B62,"F")&amp;" Females"</f>
@@ -5455,13 +5451,13 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="24.34"/>
   </cols>
@@ -7764,7 +7760,7 @@
     <row r="54" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="str">
         <f aca="false">" N = "&amp;COUNTA(A2:A53)</f>
-        <v> N = 52</v>
+        <v>N = 52</v>
       </c>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
@@ -7790,23 +7786,23 @@
       </c>
       <c r="I54" s="9" t="str">
         <f aca="false">" N = "&amp;SUM(I2:I53)</f>
-        <v> N = 48</v>
+        <v>N = 48</v>
       </c>
       <c r="J54" s="9" t="str">
         <f aca="false">" N = "&amp;SUM(J2:J53)</f>
-        <v> N = 50</v>
+        <v>N = 50</v>
       </c>
       <c r="K54" s="9" t="str">
         <f aca="false">" N = "&amp;SUM(K2:K53)</f>
-        <v> N = 41</v>
+        <v>N = 41</v>
       </c>
       <c r="L54" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(L2:L53,"3")</f>
-        <v> N = 37</v>
+        <v>N = 37</v>
       </c>
       <c r="M54" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(M2:M53,"TRUE")</f>
-        <v> N = 27</v>
+        <v>N = 27</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9572,7 +9568,7 @@
     <row r="95" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="str">
         <f aca="false">" N = "&amp;COUNTA(A55:A94)</f>
-        <v> N = 40</v>
+        <v>N = 40</v>
       </c>
       <c r="B95" s="30"/>
       <c r="C95" s="30"/>
@@ -9594,27 +9590,27 @@
       </c>
       <c r="H95" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(H55:H94,"1")</f>
-        <v> N = 33</v>
+        <v>N = 33</v>
       </c>
       <c r="I95" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(I55:I94,"1")</f>
-        <v> N = 40</v>
+        <v>N = 40</v>
       </c>
       <c r="J95" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(J55:J94,"1")</f>
-        <v> N = 38</v>
+        <v>N = 38</v>
       </c>
       <c r="K95" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(K55:K94,"1")</f>
-        <v> N = 33</v>
+        <v>N = 33</v>
       </c>
       <c r="L95" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(L55:L94,"3")</f>
-        <v> N = 32</v>
+        <v>N = 32</v>
       </c>
       <c r="M95" s="9" t="str">
         <f aca="false">" N = "&amp;COUNTIF(M55:M94,"TRUE")</f>
-        <v> N = 26</v>
+        <v>N = 26</v>
       </c>
     </row>
     <row r="65536" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14006,7 +14002,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O27" activeCellId="0" sqref="O27"/>
+      <selection pane="bottomRight" activeCell="P114" activeCellId="0" sqref="P114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14015,14 +14011,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="65" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="5" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="66" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="16" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="51.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="51.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="61.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="23" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="54.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="33" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="38" style="0" width="15.83"/>
@@ -24277,12 +24273,8 @@
       <c r="N111" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="O111" s="81" t="s">
-        <v>416</v>
-      </c>
-      <c r="P111" s="76" t="n">
-        <v>0</v>
-      </c>
+      <c r="O111" s="81"/>
+      <c r="P111" s="76"/>
       <c r="Q111" s="76"/>
       <c r="R111" s="76"/>
       <c r="S111" s="76"/>
@@ -24303,14 +24295,14 @@
       <c r="AB111" s="76"/>
       <c r="AC111" s="76"/>
       <c r="AD111" s="76" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AE111" s="76" t="n">
         <f aca="false">8*16+2</f>
         <v>130</v>
       </c>
       <c r="AF111" s="74" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AG111" s="74"/>
       <c r="AH111" s="74"/>
@@ -24544,9 +24536,7 @@
       <c r="O114" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="P114" s="76" t="n">
-        <v>0</v>
-      </c>
+      <c r="P114" s="76"/>
       <c r="Q114" s="76" t="n">
         <v>18</v>
       </c>
@@ -24595,7 +24585,7 @@
         <v>42367</v>
       </c>
       <c r="C115" s="74" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D115" s="75" t="s">
         <v>295</v>
@@ -24684,7 +24674,7 @@
         <v>42250</v>
       </c>
       <c r="C116" s="74" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D116" s="75" t="s">
         <v>295</v>
@@ -24881,69 +24871,69 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="49" t="s">
+        <v>420</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>421</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>423</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>425</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>427</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>429</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>431</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>433</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="84" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C11" s="85"/>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="86" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B12" s="87"/>
       <c r="C12" s="88"/>
@@ -24953,7 +24943,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="89" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C13" s="85"/>
     </row>
@@ -24962,7 +24952,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="89" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C14" s="85"/>
     </row>
@@ -24971,7 +24961,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="89" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C15" s="85"/>
     </row>
@@ -24980,7 +24970,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="89" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C16" s="85"/>
     </row>
@@ -24989,7 +24979,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="89" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C17" s="85"/>
     </row>
@@ -24998,7 +24988,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="89" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C18" s="85"/>
     </row>
@@ -25007,28 +24997,28 @@
         <v>7</v>
       </c>
       <c r="B19" s="89" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C19" s="85"/>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="84" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="86" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25036,7 +25026,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25044,7 +25034,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25052,7 +25042,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25060,7 +25050,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25068,7 +25058,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -25097,7 +25087,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.49"/>
@@ -25135,7 +25125,7 @@
         <v>272</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J1" s="90" t="s">
         <v>293</v>
@@ -25518,7 +25508,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K8" s="92"/>
       <c r="L8" s="59"/>
@@ -26819,7 +26809,7 @@
       <c r="K32" s="94"/>
       <c r="L32" s="59"/>
       <c r="M32" s="60" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N32" s="59"/>
       <c r="O32" s="59"/>
@@ -31318,7 +31308,7 @@
         <v>0</v>
       </c>
       <c r="J116" s="97" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K116" s="92"/>
       <c r="L116" s="59"/>
@@ -31422,7 +31412,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.17"/>
@@ -31452,7 +31442,7 @@
         <v>270</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H1" s="59"/>
       <c r="I1" s="59"/>
@@ -31731,7 +31721,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="60" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I7" s="59"/>
       <c r="J7" s="59"/>
@@ -33057,7 +33047,7 @@
         <v>1800</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F36" s="18" t="n">
         <v>1</v>
@@ -33885,7 +33875,7 @@
         <v>1800</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F54" s="18" t="n">
         <v>1</v>
@@ -36819,7 +36809,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="99" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="99" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="99" width="6.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="99" width="23.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="99" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="99" width="15"/>
   </cols>
   <sheetData>
@@ -37863,7 +37853,7 @@
         <v>59</v>
       </c>
       <c r="E52" s="99" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F52" s="99" t="n">
         <v>2</v>

</xml_diff>